<commit_message>
veritabanı os modülü eklemesi
</commit_message>
<xml_diff>
--- a/lib/usefile/irsaliye.xlsx
+++ b/lib/usefile/irsaliye.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>müşteri kodu</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>DEFTER NO</t>
-  </si>
-  <si>
-    <t>P-43-43-351</t>
   </si>
   <si>
     <t>gemi adı</t>
@@ -507,10 +504,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -526,9 +526,10 @@
     <col min="11" max="11" width="6.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="10" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" style="2" customWidth="1"/>
-    <col min="14" max="15" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="26" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="1" customWidth="1"/>
+    <col min="17" max="25" width="9.140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="1" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="20.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="22.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="11.5703125" style="1" customWidth="1"/>
@@ -1732,7 +1733,7 @@
         <v>15</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
@@ -1767,8 +1768,8 @@
         <v>0</v>
       </c>
       <c r="I19" s="8">
-        <f>AB10</f>
-        <v>0</v>
+        <f>(AB10-0.0011)</f>
+        <v>-1.1000000000000001E-3</v>
       </c>
       <c r="J19" s="9">
         <f>AB11</f>
@@ -1785,12 +1786,12 @@
         <v>21</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="AA20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
@@ -1816,7 +1817,7 @@
         <v>25</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.25">
@@ -1915,8 +1916,9 @@
       <c r="C67" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>32</v>
+      <c r="D67" s="1">
+        <f>AB23</f>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
@@ -1930,6 +1932,6 @@
     <mergeCell ref="B39:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>